<commit_message>
added mongo router and read routes, implemented CRUD for postgresql
</commit_message>
<xml_diff>
--- a/SBP_Sprint_backlog.xlsx
+++ b/SBP_Sprint_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1. (18.5.-25.5.)" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="58">
   <si>
     <t>Product backlog stavka</t>
   </si>
@@ -130,6 +130,66 @@
   </si>
   <si>
     <t>Hrvoje Zovko</t>
+  </si>
+  <si>
+    <t>Povezivanje MongoDB baze</t>
+  </si>
+  <si>
+    <t>Kreiranje frontenda za mongodb tablice</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Pravljenje axios zahtjeva</t>
+  </si>
+  <si>
+    <t>Generiranje redova tablice iz response</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>1h 30 min</t>
+  </si>
+  <si>
+    <t>Popunjavanje MongoDB baze</t>
+  </si>
+  <si>
+    <t>Spajanje na bazu</t>
+  </si>
+  <si>
+    <t>Kreiranje baze i kolekcija</t>
+  </si>
+  <si>
+    <t>Popunjavanje kolekcija</t>
+  </si>
+  <si>
+    <t>Implementacija rutera za mongodb</t>
+  </si>
+  <si>
+    <t>Implementacija rute za dobavljanje kolekcija</t>
+  </si>
+  <si>
+    <t>Implementacija rute za dobavljanje dokumenata</t>
+  </si>
+  <si>
+    <t>CRUD za PostgreSQL</t>
+  </si>
+  <si>
+    <t>Implementacija INSERT rute</t>
+  </si>
+  <si>
+    <t>Implementacija UPDATE rute</t>
+  </si>
+  <si>
+    <t>Implementacija DELETE rute</t>
+  </si>
+  <si>
+    <t>Kreiranje frontenda za akcije nad tablicom</t>
+  </si>
+  <si>
+    <t>Kreiranje frontenda za modale</t>
   </si>
 </sst>
 </file>
@@ -197,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -315,11 +375,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -348,6 +421,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,7 +433,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -666,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -709,7 +785,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -729,7 +805,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -747,8 +823,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -763,7 +839,7 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
@@ -781,7 +857,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -797,7 +873,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -805,7 +881,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -813,7 +889,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -821,7 +897,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -829,7 +905,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -845,7 +921,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -863,7 +939,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
@@ -879,7 +955,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
@@ -895,7 +971,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
@@ -911,7 +987,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8" t="s">
         <v>19</v>
       </c>
@@ -927,7 +1003,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -935,7 +1011,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -943,7 +1019,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -951,7 +1027,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -959,7 +1035,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -975,7 +1051,7 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -993,7 +1069,7 @@
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="8" t="s">
         <v>36</v>
       </c>
@@ -1009,7 +1085,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1017,7 +1093,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -1025,7 +1101,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -1033,7 +1109,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1041,7 +1117,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1049,7 +1125,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -1057,7 +1133,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1065,7 +1141,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1081,7 +1157,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -1099,7 +1175,7 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="8" t="s">
         <v>22</v>
       </c>
@@ -1115,7 +1191,7 @@
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1123,7 +1199,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -1131,7 +1207,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -1139,7 +1215,7 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1147,7 +1223,7 @@
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -1155,7 +1231,7 @@
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -1163,7 +1239,7 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -1171,7 +1247,7 @@
       <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -1194,12 +1270,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="2" customWidth="1"/>
     <col min="3" max="4" width="25.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
@@ -1235,55 +1313,105 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="A3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1291,7 +1419,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1299,7 +1427,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1307,7 +1435,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1323,31 +1451,57 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1355,7 +1509,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1363,7 +1517,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1371,7 +1525,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1379,7 +1533,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1387,7 +1541,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1395,7 +1549,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1411,55 +1565,105 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="A25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1467,7 +1671,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -1475,7 +1679,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1483,7 +1687,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1546,7 +1750,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1554,7 +1758,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1562,7 +1766,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1570,7 +1774,7 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1578,7 +1782,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1586,7 +1790,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1594,7 +1798,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1602,7 +1806,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1610,7 +1814,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1618,7 +1822,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1634,7 +1838,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1642,7 +1846,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1650,7 +1854,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1658,7 +1862,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1666,7 +1870,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1674,7 +1878,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1682,7 +1886,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1690,7 +1894,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1698,7 +1902,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1706,7 +1910,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1722,7 +1926,7 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1730,7 +1934,7 @@
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -1738,7 +1942,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1746,7 +1950,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -1754,7 +1958,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -1762,7 +1966,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1770,7 +1974,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1778,7 +1982,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -1786,7 +1990,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1794,7 +1998,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>

</xml_diff>

<commit_message>
updated final sprint backlog
</commit_message>
<xml_diff>
--- a/SBP_Sprint_backlog.xlsx
+++ b/SBP_Sprint_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1. (18.5.-25.5.)" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="91">
   <si>
     <t>Product backlog stavka</t>
   </si>
@@ -190,12 +190,111 @@
   </si>
   <si>
     <t>Kreiranje frontenda za modale</t>
+  </si>
+  <si>
+    <t>Poboljšanje PostgreSQL CRUD operacija</t>
+  </si>
+  <si>
+    <t>Mapiranje stranih kolona na frontendu</t>
+  </si>
+  <si>
+    <t>Zamjena inputa za strani id sa selectom vrijednosti iz strane tablice</t>
+  </si>
+  <si>
+    <t>Validacija inputa za partije i runde</t>
+  </si>
+  <si>
+    <t>Implementacija CRUD operacija za MongoDB</t>
+  </si>
+  <si>
+    <t>Kreiranje CRUD ruta</t>
+  </si>
+  <si>
+    <t>Renderiranje JSON formata u tablici (read only)</t>
+  </si>
+  <si>
+    <t>Renderiranje JSON formata u CRUD modalu</t>
+  </si>
+  <si>
+    <t>Implementacija CRUD operacija preko JsonTree rekurzivnog modela</t>
+  </si>
+  <si>
+    <t>Poboljšanje korisničkog sučelja</t>
+  </si>
+  <si>
+    <t>Formatiranje PostgreSQL select inputa</t>
+  </si>
+  <si>
+    <t>Kreiranje MongoDB CRUD modala</t>
+  </si>
+  <si>
+    <t>Formatiranje JSON formata u tablici</t>
+  </si>
+  <si>
+    <t>Formatiranje JSON formata u modalu</t>
+  </si>
+  <si>
+    <t>Formatiranje rekurzivnog inputa u modalu</t>
+  </si>
+  <si>
+    <t>Dodavanje indikatora za učitavanje elemenata (loading)</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Generalna ruta za sve tablice koje imaju normirana imena kolona</t>
+  </si>
+  <si>
+    <t>Ruta za mapiranje stranih ključeva i kolona (generalna)</t>
+  </si>
+  <si>
+    <t>Ruta za mapiranje stranih ključeva i kolona (specifična)</t>
+  </si>
+  <si>
+    <t>Specifična ruta za iznimne tablice (partija, runda)</t>
+  </si>
+  <si>
+    <t>Validacija samo preko frontenda</t>
+  </si>
+  <si>
+    <t>Generiranje pseudo kolona iz atributa prve razine (od svakog dokumenta u kolekciji)</t>
+  </si>
+  <si>
+    <t>NULL vrijednosti ostaju prazna polja u tablici</t>
+  </si>
+  <si>
+    <t>1h 10 min</t>
+  </si>
+  <si>
+    <t>1h 20 min</t>
+  </si>
+  <si>
+    <t>Sličan prikaz kao u read-only, samo uz pseudo kolone kao atribute i naziv dokumenta kao naziv objekta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 min </t>
+  </si>
+  <si>
+    <t>2h 20 min</t>
+  </si>
+  <si>
+    <t>Error handling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,6 +523,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -432,9 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,17 +845,17 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -776,7 +875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -784,8 +883,8 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -804,8 +903,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -822,8 +921,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
@@ -838,8 +937,8 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
@@ -856,8 +955,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -872,47 +971,47 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -920,8 +1019,8 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -938,8 +1037,8 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
@@ -954,8 +1053,8 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
@@ -970,8 +1069,8 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
@@ -986,8 +1085,8 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>19</v>
       </c>
@@ -1002,47 +1101,47 @@
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1050,8 +1149,8 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -1068,8 +1167,8 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
       <c r="B26" s="8" t="s">
         <v>36</v>
       </c>
@@ -1084,71 +1183,71 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1156,8 +1255,8 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -1174,8 +1273,8 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="13"/>
       <c r="B37" s="8" t="s">
         <v>22</v>
       </c>
@@ -1190,64 +1289,64 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="13"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="13"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -1270,21 +1369,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1312,8 +1411,8 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1330,8 +1429,8 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>50</v>
       </c>
@@ -1346,8 +1445,8 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>51</v>
       </c>
@@ -1362,24 +1461,24 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>41</v>
       </c>
@@ -1394,8 +1493,8 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>42</v>
       </c>
@@ -1410,39 +1509,39 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1450,8 +1549,8 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1468,8 +1567,8 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>47</v>
       </c>
@@ -1484,8 +1583,8 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>48</v>
       </c>
@@ -1500,63 +1599,63 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1564,8 +1663,8 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -1582,8 +1681,8 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
       <c r="B26" s="8" t="s">
         <v>54</v>
       </c>
@@ -1598,8 +1697,8 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>55</v>
       </c>
@@ -1614,8 +1713,8 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>56</v>
       </c>
@@ -1630,8 +1729,8 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>41</v>
       </c>
@@ -1646,8 +1745,8 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>57</v>
       </c>
@@ -1662,32 +1761,32 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1709,19 +1808,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="30.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1749,87 +1850,143 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1837,87 +1994,141 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+    <row r="15" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+    <row r="17" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1925,80 +2136,130 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>

</xml_diff>